<commit_message>
I modified exel_test2.xlxs file
</commit_message>
<xml_diff>
--- a/Exel _ Test2.xlsx
+++ b/Exel _ Test2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\GIT Tranining\GIT Hub\alemrepository\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACBD3611-E161-46F3-8144-DC4698937282}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62C757CE-CD8D-4508-AE66-72AC9B2760C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
   <si>
     <t>No.</t>
   </si>
@@ -58,6 +58,15 @@
   </si>
   <si>
     <t>ethiopia</t>
+  </si>
+  <si>
+    <t>alem</t>
+  </si>
+  <si>
+    <t>tsehey</t>
+  </si>
+  <si>
+    <t>GO</t>
   </si>
 </sst>
 </file>
@@ -394,7 +403,7 @@
   <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -449,13 +458,27 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="1">
+        <v>40</v>
+      </c>
+      <c r="E3" s="1">
+        <v>911140743</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>

</xml_diff>